<commit_message>
Save the Documentation File
</commit_message>
<xml_diff>
--- a/Data/Output/CompanyReport.xlsx
+++ b/Data/Output/CompanyReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravindra prasad\Documents\UiPath\GoogleSearchProcess-RE\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9D6CDE-A381-44E8-8FED-BF6738B2F387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CB74AB-9B3C-434D-8B97-C8BDC4F10130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{62C49E9F-9761-4632-BF21-6C525B5D0902}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>CompanyName</t>
   </si>
@@ -84,9 +84,6 @@
     <t>https://www.amazon.in/amazonpay/home?ref_=apay_logo_APayDashboard</t>
   </si>
   <si>
-    <t>https://www.amazon.in/events/greatindianfestival</t>
-  </si>
-  <si>
     <t>https://account.microsoft.com/account/Account</t>
   </si>
   <si>
@@ -108,52 +105,70 @@
     <t>https://www.wipro.com/en-US/</t>
   </si>
   <si>
-    <t>https://www.google.co.in/inputtools/try/</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/?hl=hi</t>
+    <t>https://translate.google.co.in/</t>
+  </si>
+  <si>
+    <t>Techmahindra</t>
+  </si>
+  <si>
+    <t>https://careers.techmahindra.com/</t>
+  </si>
+  <si>
+    <t>https://careers.techmahindra.com/CurrentOpportunity.aspx</t>
+  </si>
+  <si>
+    <t>https://www.techmahindra.com/en-in/search/?key=jobs</t>
+  </si>
+  <si>
+    <t>https://www.techmahindra.com/en-in/techmahindra-overview/</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>https://secure.verizon.com/vzauth/UI/Login</t>
+  </si>
+  <si>
+    <t>https://www.verizon.com/about/careers</t>
+  </si>
+  <si>
+    <t>https://www.verizon.com/smartphones/</t>
+  </si>
+  <si>
+    <t>https://www.verizon.com/plans/</t>
+  </si>
+  <si>
+    <t>https://www.google.co.in/maps</t>
+  </si>
+  <si>
+    <t>Dell</t>
+  </si>
+  <si>
+    <t>https://www.dell.com/en-in/shop/deals/laptop-deals</t>
+  </si>
+  <si>
+    <t>https://www.dell.com/support/home/en-in</t>
+  </si>
+  <si>
+    <t>https://www.dell.com/support/home/en-in?app=drivers</t>
+  </si>
+  <si>
+    <t>https://www.dell.com/en-in/shop/laptops-2-in-1-pcs/sc/laptops</t>
   </si>
   <si>
     <t>https://www.amazon.in/Home-Kitchen/b?ie=UTF8&amp;node=976442031</t>
   </si>
   <si>
+    <t>https://www.amazon.in/b?ie=UTF8&amp;node=7459780031</t>
+  </si>
+  <si>
     <t>https://books.google.co.in/</t>
   </si>
   <si>
-    <t>https://translate.google.co.in/</t>
-  </si>
-  <si>
-    <t>Techmahindra</t>
-  </si>
-  <si>
-    <t>https://careers.techmahindra.com/</t>
-  </si>
-  <si>
-    <t>https://careers.techmahindra.com/CurrentOpportunity.aspx</t>
-  </si>
-  <si>
-    <t>https://www.techmahindra.com/en-in/search/?key=jobs</t>
-  </si>
-  <si>
-    <t>https://www.techmahindra.com/en-in/techmahindra-overview/</t>
-  </si>
-  <si>
-    <t>Verizon</t>
-  </si>
-  <si>
-    <t>https://secure.verizon.com/vzauth/UI/Login</t>
-  </si>
-  <si>
-    <t>https://www.verizon.com/about/careers</t>
-  </si>
-  <si>
-    <t>https://www.verizon.com/smartphones/</t>
-  </si>
-  <si>
-    <t>https://www.verizon.com/plans/</t>
-  </si>
-  <si>
-    <t>https://www.microsoft.com/en-in/microsoft-teams/group-chat-software</t>
+    <t>https://news.google.co.in/</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-in/download</t>
   </si>
 </sst>
 </file>
@@ -505,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91EEA81-BEF7-4348-A3B9-7F851A8DE70E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,121 +554,138 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>